<commit_message>
Fix duplicate submit_application routes, update marketplace template, remove old handler
</commit_message>
<xml_diff>
--- a/GDARD.xlsx
+++ b/GDARD.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1725" yWindow="1725" windowWidth="21600" windowHeight="11715" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GDARD" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Products" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Users" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -67,9 +68,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -152,44 +153,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -216,32 +217,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -268,24 +251,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -297,142 +262,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -442,15 +431,63 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maize Seeds</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Agriculture</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Fertilizer X</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>120</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -460,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +563,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gerald</t>
+          <t>gaston</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -536,7 +573,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>scrypt:32768:8:1$v0Ft2VwuXc9dSusb$4de1b39fad3235bbde0e1085a9688682b4d62efe50af635c427e5c95dc282f8a08033bc3505f75fe41ba19cbc3621f59b396204df027c0f1d07af09a583ccff9</t>
+          <t>scrypt:32768:8:1$u0lmjtMdRz8jYnqn$284cda03b9a9ca4f96ef6b7bc89a3dcb38e2214911e83d7de0e8da892e1c7de16f05254f5c0b3d5c37ea188f927b7cba10aa523755326df26cef60ee3dd15841</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -545,7 +582,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -555,7 +592,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" s="3" t="n">
-        <v>45794.56855635417</v>
+        <v>45801.49542217593</v>
       </c>
     </row>
     <row r="3">
@@ -564,17 +601,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MAYY</t>
+          <t>gio</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>mayc@gmail.com</t>
+          <t>djgyanos3@gmail.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>scrypt:32768:8:1$GJ2pptFm3D600tDs$d5570dd25227b6d55bc84ffdc6979ca61a29c91f1f89c85a4fb1f818039f717e4f7569f9efbe975a7cb71104f44a499156c10d1f103c2ae0d496d1fed67819b1</t>
+          <t>scrypt:32768:8:1$DsIRoVZZNtht9zHc$d6999c54fdfba43fc8bb59ef0120dd7a5b08bad6ef68732a724e66fc5ba8aceab132e4697b38eac3f7c7a601e29ab1188437579569a2b23d999a747345ebe4dc</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -593,197 +630,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" s="3" t="n">
-        <v>45799.34651501157</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>g@g.com</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>scrypt:32768:8:1$UZG2M2DwhNfYVDDS$8f1057bee18564b19fe62c3109d2981648b149c54fac19c0026596516a80a45c4aaa29989497996784ee6bede0ded02dae12d21eb8aa5d03f312685962fd7db9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>buyer</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>pta</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" s="3" t="n">
-        <v>45799.34725371528</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>gg@gmail.com</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>scrypt:32768:8:1$uq9pTLhtcMn5c3Az$0144e2fb00ac1294322a3d9d7bb31ba37e5873ef463c1001526b06eb307268efc84f8063629f0ac2d3e117480f1ab68051b70585e82607d38b18deaafa3c9eeb</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>agent</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>CPT</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" s="3" t="n">
-        <v>45799.35372622685</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ggg@gmail.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>scrypt:32768:8:1$3VyqjHYeH1msOGH3$84221efe3e85590e8ef17e1e3cd3b52f9fcc1b62448dd2bfa03906683c0539f515386f02c12a0d01a7f138e00622953b09f0fac2c2d37a45a54b4fc4428d2c92</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>agent</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>CPT</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" s="3" t="n">
-        <v>45799.35538326389</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>gggg@gmail.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>scrypt:32768:8:1$YAq8HDhhZhP7uaoS$d6a824e768fe7335a8b60321d6ea36e1fd0be055133450608cca51a1877478e535bb7f436928dc84722617d5007aef6b609fb87d8d1b12081bc47d2699fe5eab</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>agent</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>PTA</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" s="3" t="n">
-        <v>45799.35603722222</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>itrade</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>itradeafrika@gmail.com</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>scrypt:32768:8:1$54o6ygsFR8Azx1yC$f1c2516998fa6e268e955895413be2764169a74d4c967d779c8877d9e277b70e57e3ecdaad541a644aeb09e136277cf7c708b48cdc52be5619427091a9174feb</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>agent</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" s="3" t="n">
-        <v>45799.36356195392</v>
+        <v>45801.54615556749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>